<commit_message>
Primer web scraper funcional de Mercado Libre (estoy extremadamente feliz)
</commit_message>
<xml_diff>
--- a/amazon_scraper/pokemon_prices.xlsx
+++ b/amazon_scraper/pokemon_prices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,677 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pokemon_prices</t>
+          <t>pokemon_prices 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>pokemon_reviews</t>
+          <t>pokemon_prices 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pokemon_prices 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Peluche Pikachu Pokemon Hermoso Juguete</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>59.990</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>52.240</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4.353</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Eevee Evoluciones Nintendo Game Freak 17cms</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>41.990</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>40.730</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3.394</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Squirtle Bulbasaur Gengar Regalo Colección</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>38.900</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>35.010</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>972</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Peluche Pikachu Pokemon Hermoso Juguete</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>59.990</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>52.240</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4.353</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Eevee Evoluciones Nintendo Game Freak 17cms</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>41.990</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>40.730</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3.394</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Eevee Nintendo Game Freak</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>39.990</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>35.870</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2.989</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Peluche Pikachu Charizard Y Juguete De Alta Calidad</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>64.990</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>58.491</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4.874</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Squirtle Bulbasaur Gengar Regalo Colección</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>38.900</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>35.010</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>972</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Seel Dewgong Nintendo Game Freak</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>64.990</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5.415</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2.774</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Mew Legendario Game Freak Nintendo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>36.990</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>33.291</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5.253</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Peluche Mega Charizard X Pokemon Game Freak Nintendo Regalo</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>67.990</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1.888</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1.937</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Peluche Mew Pokemon Legendario Game Freak Nintendo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>36.990</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.027</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4.049</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Peluche Togepi Pokemon Kawaii Game Freak Nintendo Regalo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>49.990</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1.388</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4.108</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Peluche Mega Charizard X Pokemon Game Freak Nintendo 25 Cms</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>64.990</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>63.040</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6.374</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Peluche Charizard Blastoise Pokemon 40cm X 39cm Grande</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>71.900</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>69.743</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1.481</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Cubone Marowak Nintendo Game Freak Juguete</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>52.990</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>48.591</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>5.253</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Peluche Cubone Pokemon Tierno Game Freak Nintendo 16,5 Cms</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>52.990</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1.471</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1.751</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Gengar Peluche Pokémon 36 Cm Alto Excelente Calidad</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>58.000</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>49.300</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2.989</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Peluche Bulbasaur Pokemon Planta Game Freak Nintendo Regalo</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>59.990</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1.666</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>4.874</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Peluche Lapras Tipo Agua Nintendo Game Freak Pokemon Regalo</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>51.990</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1.444</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>4.124</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Mewtwo Mew Nintendo Game Freak Juguete</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>84.990</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>76.491</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5.250</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Peluche Blastoise Tipo Agua Game Freak Nintendo Regalo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>54.990</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>53.340</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2.550</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Pikachu Mega Charizard X Nintendo Game Freak</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>64.990</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>63.040</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>897</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Peluche Evee Evoluciones Pokemon Game Freak Nintendo Kawaii</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>44.990</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1.249</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2.559</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Peluche Pikachu Mega Charizard X Nintendo Game Freak Pokemon</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>64.990</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>63.040</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1.052</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Peluche Snorlax Pokemon Kawaii Game Freak Nintendo Regalo</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>34.990</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>971</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3.629</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Peluches Pokemon Gengar Pokemon 34cm X 34cm Juguete</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>44.900</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1.247</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>5.359</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Peluche Charmander Inicial Fuego Nintendo Game Freak Pokemon</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>59.990</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1.666</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1.111</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Peluche Llavero Pokémon Pikachu Charmander Squirtle Eevee</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>20.000</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>555</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>3.895</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Peluche Pokemon Eevee Nintendo Game Freak</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>39.990</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>35.870</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4.874</t>
         </is>
       </c>
     </row>

</xml_diff>